<commit_message>
Entrega final. Falta ultimas actualizaciones de las ultimas actividades.
</commit_message>
<xml_diff>
--- a/B2-1/BEBA/Actividades/BEBA_U3_A3_BERC.xlsx
+++ b/B2-1/BEBA/Actividades/BEBA_U3_A3_BERC.xlsx
@@ -86,9 +86,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -233,7 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,7 +261,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -296,7 +295,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -309,6 +308,262 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$F$3:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Media</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Moda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mediana</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Varianza</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Desviacion estandar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.185</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.244</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="18677156"/>
+        <c:axId val="40355306"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="18677156"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="40355306"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="40355306"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18677156"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11880</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>98280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146520</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="583200" y="1864080"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -317,10 +572,10 @@
   <dimension ref="A2:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.41"/>
@@ -328,7 +583,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" s="4" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -500,5 +755,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>